<commit_message>
added final two games, fixed results of four older games
</commit_message>
<xml_diff>
--- a/raw/Літній Мажор результати.xlsx
+++ b/raw/Літній Мажор результати.xlsx
@@ -192,9 +192,6 @@
     <t>Прозорі Зумери</t>
   </si>
   <si>
-    <t>Андрюша</t>
-  </si>
-  <si>
     <t>Назва команди</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Комети (ЩДКоти)</t>
+  </si>
+  <si>
+    <t>Легіон</t>
   </si>
 </sst>
 </file>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,31 +698,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1829,7 +1829,7 @@
     </row>
     <row r="40" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>54</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="43" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>44</v>

</xml_diff>